<commit_message>
primeiro eq conceito A
</commit_message>
<xml_diff>
--- a/uerj-provas (version 1).xlsx
+++ b/uerj-provas (version 1).xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jory\Desktop\misc\uerj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDAEF14-F87C-4C2E-942B-6D14B1010916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907BB9FE-3AE3-4C05-92FD-4FCD1DBE78B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="16200" activeTab="1" xr2:uid="{1848C7D1-DA3E-4FAE-A765-5535C3F621E3}"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="16200" xr2:uid="{B0F7470C-BA10-478C-AEC0-BA65017C653B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" activeTab="2" xr2:uid="{1848C7D1-DA3E-4FAE-A765-5535C3F621E3}"/>
   </bookViews>
   <sheets>
     <sheet name="2024.1" sheetId="2" r:id="rId1"/>
     <sheet name="2024.2" sheetId="1" r:id="rId2"/>
+    <sheet name="2025.1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="110">
   <si>
     <t>UERJ 2024 2º EQ</t>
   </si>
@@ -382,6 +382,12 @@
       </rPr>
       <t xml:space="preserve"> - Plano cartesiano</t>
     </r>
+  </si>
+  <si>
+    <t>UERJ 2025 1º EQ</t>
+  </si>
+  <si>
+    <t>MARQUEI 2</t>
   </si>
 </sst>
 </file>
@@ -557,6 +563,7 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -581,7 +588,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,8 +596,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFFF66"/>
       <color rgb="FFFF7C80"/>
-      <color rgb="FFFFFF66"/>
     </mruColors>
   </colors>
   <extLst>
@@ -927,9 +933,6 @@
     <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="F62" sqref="F62"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="1">
-      <selection activeCell="E30" sqref="E30"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -939,13 +942,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
@@ -963,7 +966,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2">
@@ -980,7 +983,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="2">
         <v>2</v>
       </c>
@@ -998,7 +1001,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="2">
         <v>3</v>
       </c>
@@ -1013,7 +1016,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="2">
         <v>4</v>
       </c>
@@ -1028,7 +1031,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="2">
         <v>5</v>
       </c>
@@ -1043,7 +1046,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="2">
         <v>6</v>
       </c>
@@ -1058,7 +1061,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="2">
         <v>7</v>
       </c>
@@ -1073,7 +1076,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="2">
         <v>8</v>
       </c>
@@ -1088,7 +1091,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="20" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="4">
@@ -1108,7 +1111,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="4">
         <v>10</v>
       </c>
@@ -1123,7 +1126,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="4">
         <v>11</v>
       </c>
@@ -1138,7 +1141,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
+      <c r="A14" s="20"/>
       <c r="B14" s="4">
         <v>12</v>
       </c>
@@ -1153,7 +1156,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="4">
         <v>13</v>
       </c>
@@ -1171,7 +1174,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="20"/>
       <c r="B16" s="4">
         <v>14</v>
       </c>
@@ -1186,7 +1189,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="4">
         <v>15</v>
       </c>
@@ -1201,7 +1204,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="4">
         <v>16</v>
       </c>
@@ -1216,7 +1219,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="4">
         <v>17</v>
       </c>
@@ -1231,7 +1234,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="4">
         <v>18</v>
       </c>
@@ -1246,7 +1249,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
+      <c r="A21" s="20"/>
       <c r="B21" s="4">
         <v>19</v>
       </c>
@@ -1267,7 +1270,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="4">
         <v>20</v>
       </c>
@@ -1282,7 +1285,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
+      <c r="A23" s="20"/>
       <c r="B23" s="4">
         <v>21</v>
       </c>
@@ -1297,7 +1300,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
+      <c r="A24" s="20"/>
       <c r="B24" s="4">
         <v>22</v>
       </c>
@@ -1312,7 +1315,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="21" t="s">
         <v>10</v>
       </c>
       <c r="B25" s="5">
@@ -1329,7 +1332,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="5">
         <v>24</v>
       </c>
@@ -1344,7 +1347,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="5">
         <v>25</v>
       </c>
@@ -1359,7 +1362,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="5">
         <v>26</v>
       </c>
@@ -1374,7 +1377,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="5">
         <v>27</v>
       </c>
@@ -1389,7 +1392,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="22" t="s">
         <v>11</v>
       </c>
       <c r="B30" s="6">
@@ -1401,12 +1404,12 @@
       <c r="D30" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E30" s="23" t="s">
+      <c r="E30" s="15" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
+      <c r="A31" s="22"/>
       <c r="B31" s="6">
         <v>29</v>
       </c>
@@ -1421,7 +1424,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
+      <c r="A32" s="22"/>
       <c r="B32" s="6">
         <v>30</v>
       </c>
@@ -1436,7 +1439,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="21"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="6">
         <v>31</v>
       </c>
@@ -1451,7 +1454,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="21"/>
+      <c r="A34" s="22"/>
       <c r="B34" s="6">
         <v>32</v>
       </c>
@@ -1466,7 +1469,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
+      <c r="A35" s="22"/>
       <c r="B35" s="6">
         <v>33</v>
       </c>
@@ -1481,7 +1484,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="21"/>
+      <c r="A36" s="22"/>
       <c r="B36" s="6">
         <v>34</v>
       </c>
@@ -1491,12 +1494,12 @@
       <c r="D36" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E36" s="23" t="s">
+      <c r="E36" s="15" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="22" t="s">
+      <c r="A37" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B37" s="7">
@@ -1516,7 +1519,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
+      <c r="A38" s="23"/>
       <c r="B38" s="7">
         <v>36</v>
       </c>
@@ -1531,7 +1534,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
+      <c r="A39" s="23"/>
       <c r="B39" s="7">
         <v>37</v>
       </c>
@@ -1546,7 +1549,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
+      <c r="A40" s="23"/>
       <c r="B40" s="7">
         <v>38</v>
       </c>
@@ -1561,7 +1564,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
+      <c r="A41" s="23"/>
       <c r="B41" s="7">
         <v>39</v>
       </c>
@@ -1576,7 +1579,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
+      <c r="A42" s="23"/>
       <c r="B42" s="7">
         <v>40</v>
       </c>
@@ -1591,7 +1594,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
+      <c r="A43" s="23"/>
       <c r="B43" s="7">
         <v>41</v>
       </c>
@@ -1609,7 +1612,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
+      <c r="A44" s="23"/>
       <c r="B44" s="7">
         <v>42</v>
       </c>
@@ -1624,7 +1627,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
+      <c r="A45" s="23"/>
       <c r="B45" s="7">
         <v>43</v>
       </c>
@@ -1639,7 +1642,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="22"/>
+      <c r="A46" s="23"/>
       <c r="B46" s="7">
         <v>44</v>
       </c>
@@ -1654,7 +1657,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="22"/>
+      <c r="A47" s="23"/>
       <c r="B47" s="7">
         <v>45</v>
       </c>
@@ -1669,7 +1672,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="22"/>
+      <c r="A48" s="23"/>
       <c r="B48" s="7">
         <v>46</v>
       </c>
@@ -1684,7 +1687,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B49" s="8">
@@ -1701,7 +1704,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="15"/>
+      <c r="A50" s="16"/>
       <c r="B50" s="8">
         <v>48</v>
       </c>
@@ -1716,7 +1719,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="15"/>
+      <c r="A51" s="16"/>
       <c r="B51" s="8">
         <v>49</v>
       </c>
@@ -1731,7 +1734,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="15"/>
+      <c r="A52" s="16"/>
       <c r="B52" s="8">
         <v>50</v>
       </c>
@@ -1746,7 +1749,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="15"/>
+      <c r="A53" s="16"/>
       <c r="B53" s="8">
         <v>51</v>
       </c>
@@ -1761,7 +1764,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="15"/>
+      <c r="A54" s="16"/>
       <c r="B54" s="8">
         <v>52</v>
       </c>
@@ -1776,7 +1779,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="15"/>
+      <c r="A55" s="16"/>
       <c r="B55" s="8">
         <v>53</v>
       </c>
@@ -1791,7 +1794,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
+      <c r="A56" s="16"/>
       <c r="B56" s="8">
         <v>54</v>
       </c>
@@ -1809,7 +1812,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="15"/>
+      <c r="A57" s="16"/>
       <c r="B57" s="8">
         <v>55</v>
       </c>
@@ -1824,7 +1827,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="15"/>
+      <c r="A58" s="16"/>
       <c r="B58" s="8">
         <v>56</v>
       </c>
@@ -1839,7 +1842,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="15"/>
+      <c r="A59" s="16"/>
       <c r="B59" s="8">
         <v>57</v>
       </c>
@@ -1854,7 +1857,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="15"/>
+      <c r="A60" s="16"/>
       <c r="B60" s="8">
         <v>58</v>
       </c>
@@ -1869,7 +1872,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="15"/>
+      <c r="A61" s="16"/>
       <c r="B61" s="8">
         <v>59</v>
       </c>
@@ -1887,7 +1890,7 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="15"/>
+      <c r="A62" s="16"/>
       <c r="B62" s="8">
         <v>60</v>
       </c>
@@ -1919,11 +1922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA600253-52D9-4B27-B274-12A21FB25328}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection sqref="A1:E1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A49" sqref="A1:E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,13 +1934,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="9"/>
@@ -1958,7 +1958,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="2">
@@ -1976,7 +1976,7 @@
       <c r="F3" s="12"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="2">
         <v>2</v>
       </c>
@@ -1991,7 +1991,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="2">
         <v>3</v>
       </c>
@@ -2006,7 +2006,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="2">
         <v>4</v>
       </c>
@@ -2021,7 +2021,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="2">
         <v>5</v>
       </c>
@@ -2036,7 +2036,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="2">
         <v>6</v>
       </c>
@@ -2051,7 +2051,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="2">
         <v>7</v>
       </c>
@@ -2066,7 +2066,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="2">
         <v>8</v>
       </c>
@@ -2081,7 +2081,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="20" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="4">
@@ -2098,7 +2098,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="4">
         <v>10</v>
       </c>
@@ -2113,7 +2113,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
+      <c r="A13" s="20"/>
       <c r="B13" s="4">
         <v>11</v>
       </c>
@@ -2128,7 +2128,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
+      <c r="A14" s="20"/>
       <c r="B14" s="4">
         <v>12</v>
       </c>
@@ -2143,7 +2143,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
+      <c r="A15" s="20"/>
       <c r="B15" s="4">
         <v>13</v>
       </c>
@@ -2161,7 +2161,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="19"/>
+      <c r="A16" s="20"/>
       <c r="B16" s="4">
         <v>14</v>
       </c>
@@ -2176,7 +2176,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="19"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="4">
         <v>15</v>
       </c>
@@ -2191,7 +2191,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="19"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="4">
         <v>16</v>
       </c>
@@ -2209,7 +2209,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="19"/>
+      <c r="A19" s="20"/>
       <c r="B19" s="4">
         <v>17</v>
       </c>
@@ -2224,7 +2224,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="19"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="4">
         <v>18</v>
       </c>
@@ -2239,7 +2239,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="19"/>
+      <c r="A21" s="20"/>
       <c r="B21" s="4">
         <v>19</v>
       </c>
@@ -2254,7 +2254,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="19"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="4">
         <v>20</v>
       </c>
@@ -2272,7 +2272,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
+      <c r="A23" s="20"/>
       <c r="B23" s="4">
         <v>21</v>
       </c>
@@ -2287,7 +2287,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
+      <c r="A24" s="20"/>
       <c r="B24" s="4">
         <v>22</v>
       </c>
@@ -2305,7 +2305,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="21" t="s">
         <v>10</v>
       </c>
       <c r="B25" s="5">
@@ -2322,7 +2322,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="5">
         <v>24</v>
       </c>
@@ -2337,7 +2337,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="20"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="5">
         <v>25</v>
       </c>
@@ -2352,7 +2352,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="20"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="5">
         <v>26</v>
       </c>
@@ -2367,7 +2367,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="20"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="5">
         <v>27</v>
       </c>
@@ -2382,7 +2382,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="21" t="s">
+      <c r="A30" s="22" t="s">
         <v>11</v>
       </c>
       <c r="B30" s="6">
@@ -2399,7 +2399,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="21"/>
+      <c r="A31" s="22"/>
       <c r="B31" s="6">
         <v>29</v>
       </c>
@@ -2414,7 +2414,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="21"/>
+      <c r="A32" s="22"/>
       <c r="B32" s="6">
         <v>30</v>
       </c>
@@ -2429,7 +2429,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="21"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="6">
         <v>31</v>
       </c>
@@ -2439,12 +2439,12 @@
       <c r="D33" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E33" s="23" t="s">
+      <c r="E33" s="15" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="21"/>
+      <c r="A34" s="22"/>
       <c r="B34" s="6">
         <v>32</v>
       </c>
@@ -2459,7 +2459,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="21"/>
+      <c r="A35" s="22"/>
       <c r="B35" s="6">
         <v>33</v>
       </c>
@@ -2469,12 +2469,12 @@
       <c r="D35" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E35" s="23" t="s">
+      <c r="E35" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="21"/>
+      <c r="A36" s="22"/>
       <c r="B36" s="6">
         <v>34</v>
       </c>
@@ -2484,12 +2484,12 @@
       <c r="D36" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E36" s="23" t="s">
+      <c r="E36" s="15" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="22" t="s">
+      <c r="A37" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B37" s="7">
@@ -2506,7 +2506,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="22"/>
+      <c r="A38" s="23"/>
       <c r="B38" s="7">
         <v>36</v>
       </c>
@@ -2521,7 +2521,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="22"/>
+      <c r="A39" s="23"/>
       <c r="B39" s="7">
         <v>37</v>
       </c>
@@ -2536,7 +2536,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="22"/>
+      <c r="A40" s="23"/>
       <c r="B40" s="7">
         <v>38</v>
       </c>
@@ -2554,7 +2554,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="22"/>
+      <c r="A41" s="23"/>
       <c r="B41" s="7">
         <v>39</v>
       </c>
@@ -2569,7 +2569,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="22"/>
+      <c r="A42" s="23"/>
       <c r="B42" s="7">
         <v>40</v>
       </c>
@@ -2584,7 +2584,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="22"/>
+      <c r="A43" s="23"/>
       <c r="B43" s="7">
         <v>41</v>
       </c>
@@ -2599,7 +2599,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="22"/>
+      <c r="A44" s="23"/>
       <c r="B44" s="7">
         <v>42</v>
       </c>
@@ -2614,7 +2614,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="22"/>
+      <c r="A45" s="23"/>
       <c r="B45" s="7">
         <v>43</v>
       </c>
@@ -2629,7 +2629,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="22"/>
+      <c r="A46" s="23"/>
       <c r="B46" s="7">
         <v>44</v>
       </c>
@@ -2647,7 +2647,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="22"/>
+      <c r="A47" s="23"/>
       <c r="B47" s="7">
         <v>45</v>
       </c>
@@ -2662,7 +2662,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="22"/>
+      <c r="A48" s="23"/>
       <c r="B48" s="7">
         <v>46</v>
       </c>
@@ -2680,7 +2680,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="16" t="s">
         <v>13</v>
       </c>
       <c r="B49" s="8">
@@ -2697,7 +2697,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="15"/>
+      <c r="A50" s="16"/>
       <c r="B50" s="8">
         <v>48</v>
       </c>
@@ -2715,7 +2715,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="15"/>
+      <c r="A51" s="16"/>
       <c r="B51" s="8">
         <v>49</v>
       </c>
@@ -2733,7 +2733,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="15"/>
+      <c r="A52" s="16"/>
       <c r="B52" s="8">
         <v>50</v>
       </c>
@@ -2748,7 +2748,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="15"/>
+      <c r="A53" s="16"/>
       <c r="B53" s="8">
         <v>51</v>
       </c>
@@ -2763,7 +2763,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="15"/>
+      <c r="A54" s="16"/>
       <c r="B54" s="8">
         <v>52</v>
       </c>
@@ -2781,7 +2781,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="15"/>
+      <c r="A55" s="16"/>
       <c r="B55" s="8">
         <v>53</v>
       </c>
@@ -2796,7 +2796,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="15"/>
+      <c r="A56" s="16"/>
       <c r="B56" s="8">
         <v>54</v>
       </c>
@@ -2811,7 +2811,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="15"/>
+      <c r="A57" s="16"/>
       <c r="B57" s="8">
         <v>55</v>
       </c>
@@ -2826,7 +2826,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="15"/>
+      <c r="A58" s="16"/>
       <c r="B58" s="8">
         <v>56</v>
       </c>
@@ -2841,7 +2841,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" s="15"/>
+      <c r="A59" s="16"/>
       <c r="B59" s="8">
         <v>57</v>
       </c>
@@ -2856,7 +2856,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" s="15"/>
+      <c r="A60" s="16"/>
       <c r="B60" s="8">
         <v>58</v>
       </c>
@@ -2871,7 +2871,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="15"/>
+      <c r="A61" s="16"/>
       <c r="B61" s="8">
         <v>59</v>
       </c>
@@ -2886,7 +2886,7 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" s="15"/>
+      <c r="A62" s="16"/>
       <c r="B62" s="8">
         <v>60</v>
       </c>
@@ -2915,4 +2915,848 @@
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AD40933-239C-4498-8E5C-3DCDAE84956A}">
+  <dimension ref="A1:E62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="19"/>
+      <c r="B4" s="2">
+        <v>2</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="19"/>
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="19"/>
+      <c r="B6" s="2">
+        <v>4</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="19"/>
+      <c r="B7" s="2">
+        <v>5</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="19"/>
+      <c r="B8" s="2">
+        <v>6</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="19"/>
+      <c r="B9" s="2">
+        <v>7</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
+      <c r="B10" s="2">
+        <v>8</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4">
+        <v>9</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
+      <c r="B12" s="4">
+        <v>10</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
+      <c r="B13" s="4">
+        <v>11</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
+      <c r="B14" s="4">
+        <v>12</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
+      <c r="B15" s="4">
+        <v>13</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
+      <c r="B16" s="4">
+        <v>14</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
+      <c r="B17" s="4">
+        <v>15</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
+      <c r="B18" s="4">
+        <v>16</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
+      <c r="B19" s="4">
+        <v>17</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
+      <c r="B20" s="4">
+        <v>18</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="20"/>
+      <c r="B21" s="4">
+        <v>19</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
+      <c r="B22" s="4">
+        <v>20</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
+      <c r="B23" s="4">
+        <v>21</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="20"/>
+      <c r="B24" s="4">
+        <v>22</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="5">
+        <v>23</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="21"/>
+      <c r="B26" s="5">
+        <v>24</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="21"/>
+      <c r="B27" s="5">
+        <v>25</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="21"/>
+      <c r="B28" s="5">
+        <v>26</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="21"/>
+      <c r="B29" s="5">
+        <v>27</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B30" s="6">
+        <v>28</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="22"/>
+      <c r="B31" s="6">
+        <v>29</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="22"/>
+      <c r="B32" s="6">
+        <v>30</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="22"/>
+      <c r="B33" s="6">
+        <v>31</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" s="15"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="22"/>
+      <c r="B34" s="6">
+        <v>32</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="22"/>
+      <c r="B35" s="6">
+        <v>33</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E35" s="15"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="22"/>
+      <c r="B36" s="6">
+        <v>34</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E36" s="15"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="7">
+        <v>35</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="23"/>
+      <c r="B38" s="7">
+        <v>36</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="23"/>
+      <c r="B39" s="7">
+        <v>37</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="23"/>
+      <c r="B40" s="7">
+        <v>38</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="23"/>
+      <c r="B41" s="7">
+        <v>39</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="23"/>
+      <c r="B42" s="7">
+        <v>40</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="23"/>
+      <c r="B43" s="7">
+        <v>41</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="23"/>
+      <c r="B44" s="7">
+        <v>42</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="23"/>
+      <c r="B45" s="7">
+        <v>43</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="23"/>
+      <c r="B46" s="7">
+        <v>44</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="23"/>
+      <c r="B47" s="7">
+        <v>45</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="23"/>
+      <c r="B48" s="7">
+        <v>46</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B49" s="8">
+        <v>47</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="16"/>
+      <c r="B50" s="8">
+        <v>48</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="16"/>
+      <c r="B51" s="8">
+        <v>49</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="16"/>
+      <c r="B52" s="8">
+        <v>50</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="16"/>
+      <c r="B53" s="8">
+        <v>51</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="16"/>
+      <c r="B54" s="8">
+        <v>52</v>
+      </c>
+      <c r="C54" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="16"/>
+      <c r="B55" s="8">
+        <v>53</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="16"/>
+      <c r="B56" s="8">
+        <v>54</v>
+      </c>
+      <c r="C56" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="16"/>
+      <c r="B57" s="8">
+        <v>55</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="16"/>
+      <c r="B58" s="8">
+        <v>56</v>
+      </c>
+      <c r="C58" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="16"/>
+      <c r="B59" s="8">
+        <v>57</v>
+      </c>
+      <c r="C59" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="16"/>
+      <c r="B60" s="8">
+        <v>58</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E60" s="1"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="16"/>
+      <c r="B61" s="8">
+        <v>59</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E61" s="1"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="16"/>
+      <c r="B62" s="8">
+        <v>60</v>
+      </c>
+      <c r="C62" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E62" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A49:A62"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="A11:A24"/>
+    <mergeCell ref="A25:A29"/>
+    <mergeCell ref="A30:A36"/>
+    <mergeCell ref="A37:A48"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>